<commit_message>
features for updated outcome measures
</commit_message>
<xml_diff>
--- a/sample settings.xlsx
+++ b/sample settings.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\SASA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C23DE56-6D9D-4373-A409-C9349CE2B6A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFC5031B-DD1A-4830-AC48-0FBBD60AAADF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{EE0EDC0E-EB97-4793-B5E3-A66C2E897836}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>filename</t>
   </si>
@@ -91,6 +91,15 @@
   </si>
   <si>
     <t>night duration round up within (minutes)</t>
+  </si>
+  <si>
+    <t>expected_sampling_rate (sec)</t>
+  </si>
+  <si>
+    <t>desat severe threshold</t>
+  </si>
+  <si>
+    <t>artifact duration threshold (sec)</t>
   </si>
 </sst>
 </file>
@@ -463,10 +472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3353DA1-A2EE-4C42-B504-14E6C68C02F6}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -500,74 +509,98 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B4">
-        <v>-5</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B5">
-        <v>10</v>
+        <v>-10</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6">
-        <v>30</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7">
-        <v>10</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B9">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="1">
-        <v>0.875</v>
+        <v>16</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="1">
+        <v>0.875</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B14" s="1">
         <v>0.29166666666666669</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added note for SB176
</commit_message>
<xml_diff>
--- a/sample settings.xlsx
+++ b/sample settings.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\SASA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFC5031B-DD1A-4830-AC48-0FBBD60AAADF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC73FC48-9D03-437F-96FD-E3AC922CF802}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{EE0EDC0E-EB97-4793-B5E3-A66C2E897836}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" activeTab="1" xr2:uid="{EE0EDC0E-EB97-4793-B5E3-A66C2E897836}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
-    <sheet name="file time fix" sheetId="2" r:id="rId2"/>
+    <sheet name="notes" sheetId="3" r:id="rId2"/>
+    <sheet name="file time fix" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>filename</t>
   </si>
@@ -100,6 +101,9 @@
   </si>
   <si>
     <t>artifact duration threshold (sec)</t>
+  </si>
+  <si>
+    <t>SB176 header needed to be corrected to match standard style</t>
   </si>
 </sst>
 </file>
@@ -474,16 +478,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3353DA1-A2EE-4C42-B504-14E6C68C02F6}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -491,7 +495,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -499,7 +503,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -507,7 +511,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -515,7 +519,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -523,7 +527,7 @@
         <v>-10</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -531,7 +535,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -539,7 +543,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -547,7 +551,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -555,7 +559,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -563,7 +567,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -571,7 +575,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -579,7 +583,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -587,7 +591,7 @@
         <v>0.875</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -595,7 +599,7 @@
         <v>0.29166666666666669</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -609,6 +613,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B3348F0-8005-40BC-BA97-561D71BC7EB6}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F57471AF-BCE1-4DE2-BF97-13478AB74FD7}">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -616,9 +640,9 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -629,7 +653,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -640,7 +664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>

</xml_diff>